<commit_message>
Adiciona o partido dos candidatos na planilha
</commit_message>
<xml_diff>
--- a/2018/Centro-Oeste/DF/resultado.xlsx
+++ b/2018/Centro-Oeste/DF/resultado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J192"/>
+  <dimension ref="A1:N192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,12 +476,32 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>DS_ESTADO_CIVIL</t>
+          <t>DS_ESTADO_CIVIL_x</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>DS_GRAU_INSTRUCAO</t>
+          <t>DS_GRAU_INSTRUCAO_x</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>DS_ESTADO_CIVIL_y</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>DS_GRAU_INSTRUCAO_y</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>SQ_CANDIDATO</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>SG_PARTIDO</t>
         </is>
       </c>
     </row>
@@ -534,6 +554,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>70000602344</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -584,6 +622,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>70000602345</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -634,6 +690,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>70000602346</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -684,6 +758,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>70000602347</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -734,6 +826,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>70000602348</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -784,6 +894,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>70000602349</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>NOVO</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -834,6 +962,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>70000602708</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -884,6 +1030,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>70000602709</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -934,6 +1098,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>70000602710</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -984,6 +1166,24 @@
           <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
         </is>
       </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>70000602711</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1034,6 +1234,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>70000602712</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1084,6 +1302,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>70000602713</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1134,6 +1370,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>70000602714</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1184,6 +1438,24 @@
           <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
         </is>
       </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>70000602715</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1234,6 +1506,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>70000602716</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1284,6 +1574,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>70000602717</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>PCB</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1334,6 +1642,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>70000602718</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1384,6 +1710,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>70000602719</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1434,6 +1778,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>70000602720</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1484,6 +1846,24 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="M21" t="n">
+        <v>70000602721</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1534,6 +1914,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M22" t="n">
+        <v>70000602722</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1584,6 +1982,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>70000602723</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1634,6 +2050,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M24" t="n">
+        <v>70000605783</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>PSTU</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1684,6 +2118,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M25" t="n">
+        <v>70000610834</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1734,6 +2186,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
+        <v>70000610835</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1784,6 +2254,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M27" t="n">
+        <v>70000610836</v>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1834,6 +2322,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M28" t="n">
+        <v>70000610837</v>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1884,6 +2390,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M29" t="n">
+        <v>70000610838</v>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1934,6 +2458,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M30" t="n">
+        <v>70000610839</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1984,6 +2526,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
+        <v>70000610840</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2034,6 +2594,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M32" t="n">
+        <v>70000610841</v>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2084,6 +2662,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M33" t="n">
+        <v>70000610842</v>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2134,6 +2730,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
+        <v>70000610843</v>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2184,6 +2798,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
+        <v>70000610844</v>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2234,6 +2866,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>70000610849</v>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2284,6 +2934,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M37" t="n">
+        <v>70000610850</v>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2334,6 +3002,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>SEPARADO(A) JUDICIALMENTE</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
+        <v>70000610851</v>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2384,6 +3070,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
+        <v>70000610852</v>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2434,6 +3138,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>SEPARADO(A) JUDICIALMENTE</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M40" t="n">
+        <v>70000610853</v>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2484,6 +3206,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M41" t="n">
+        <v>70000614417</v>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2534,6 +3274,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M42" t="n">
+        <v>70000614418</v>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>PC do B</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2584,6 +3342,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M43" t="n">
+        <v>70000614419</v>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2634,6 +3410,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M44" t="n">
+        <v>70000614420</v>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2684,6 +3478,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M45" t="n">
+        <v>70000614421</v>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2734,6 +3546,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
+        <v>70000614422</v>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2784,6 +3614,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M47" t="n">
+        <v>70000614423</v>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2834,6 +3682,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M48" t="n">
+        <v>70000614424</v>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>PC do B</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2884,6 +3750,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M49" t="n">
+        <v>70000614425</v>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2934,6 +3818,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M50" t="n">
+        <v>70000614426</v>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2984,6 +3886,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M51" t="n">
+        <v>70000614427</v>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3034,6 +3954,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M52" t="n">
+        <v>70000614428</v>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3084,6 +4022,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>SEPARADO(A) JUDICIALMENTE</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M53" t="n">
+        <v>70000614429</v>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3134,6 +4090,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M54" t="n">
+        <v>70000614430</v>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>REDE</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3184,6 +4158,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M55" t="n">
+        <v>70000614431</v>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3234,6 +4226,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M56" t="n">
+        <v>70000614432</v>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3284,6 +4294,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>VIÚVO(A)</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M57" t="n">
+        <v>70000614519</v>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3334,6 +4362,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M58" t="n">
+        <v>70000614520</v>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3384,6 +4430,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M59" t="n">
+        <v>70000614521</v>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>MDB</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3434,6 +4498,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M60" t="n">
+        <v>70000614522</v>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3484,6 +4566,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M61" t="n">
+        <v>70000614523</v>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3534,6 +4634,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M62" t="n">
+        <v>70000614524</v>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3584,6 +4702,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M63" t="n">
+        <v>70000614525</v>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>AVANTE</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3634,6 +4770,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M64" t="n">
+        <v>70000614526</v>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>AVANTE</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3684,6 +4838,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M65" t="n">
+        <v>70000614527</v>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>AVANTE</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3734,6 +4906,24 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="M66" t="n">
+        <v>70000614528</v>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>AVANTE</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3784,6 +4974,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M67" t="n">
+        <v>70000614529</v>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>AVANTE</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3834,6 +5042,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M68" t="n">
+        <v>70000614530</v>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>AVANTE</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3884,6 +5110,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M69" t="n">
+        <v>70000614531</v>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>AVANTE</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3934,6 +5178,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M70" t="n">
+        <v>70000614532</v>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>AVANTE</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3984,6 +5246,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M71" t="n">
+        <v>70000614533</v>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>PP</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -4034,6 +5314,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M72" t="n">
+        <v>70000614534</v>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>PP</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -4084,6 +5382,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M73" t="n">
+        <v>70000614972</v>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -4134,6 +5450,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M74" t="n">
+        <v>70000614973</v>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4184,6 +5518,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M75" t="n">
+        <v>70000614974</v>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4234,6 +5586,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>70000614976</v>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4284,6 +5654,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M77" t="n">
+        <v>70000614977</v>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4334,6 +5722,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M78" t="n">
+        <v>70000614980</v>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4384,6 +5790,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>70000614988</v>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4434,6 +5858,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>70000614989</v>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4484,6 +5926,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>70000615000</v>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4534,6 +5994,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>70000615017</v>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4584,6 +6062,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
+        <v>70000615018</v>
+      </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -4634,6 +6130,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>70000615019</v>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -4684,6 +6198,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>70000615020</v>
+      </c>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -4734,6 +6266,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M86" t="n">
+        <v>70000615021</v>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -4784,6 +6334,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M87" t="n">
+        <v>70000615022</v>
+      </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4834,6 +6402,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M88" t="n">
+        <v>70000615040</v>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4884,6 +6470,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>70000616401</v>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>PCO</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4934,6 +6538,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
+        <v>70000616402</v>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>PCO</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4984,6 +6606,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M91" t="n">
+        <v>70000616404</v>
+      </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>PCO</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -5034,6 +6674,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M92" t="n">
+        <v>70000616405</v>
+      </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>PCO</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -5084,6 +6742,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M93" t="n">
+        <v>70000618958</v>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>PRB</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -5134,6 +6810,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M94" t="n">
+        <v>70000618959</v>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -5184,6 +6878,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M95" t="n">
+        <v>70000618960</v>
+      </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -5234,6 +6946,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M96" t="n">
+        <v>70000618961</v>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -5284,6 +7014,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M97" t="n">
+        <v>70000618962</v>
+      </c>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5334,6 +7082,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M98" t="n">
+        <v>70000618963</v>
+      </c>
+      <c r="N98" t="inlineStr">
+        <is>
+          <t>PRB</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -5384,6 +7150,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M99" t="n">
+        <v>70000618964</v>
+      </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>SOLIDARIEDADE</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -5434,6 +7218,24 @@
           <t>ENSINO MÉDIO INCOMPLETO</t>
         </is>
       </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M100" t="n">
+        <v>70000618965</v>
+      </c>
+      <c r="N100" t="inlineStr">
+        <is>
+          <t>PSD</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -5484,6 +7286,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M101" t="n">
+        <v>70000618966</v>
+      </c>
+      <c r="N101" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -5534,6 +7354,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M102" t="n">
+        <v>70000618967</v>
+      </c>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -5584,6 +7422,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M103" t="n">
+        <v>70000618968</v>
+      </c>
+      <c r="N103" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -5634,6 +7490,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M104" t="n">
+        <v>70000618969</v>
+      </c>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>PODE</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -5684,6 +7558,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M105" t="n">
+        <v>70000618970</v>
+      </c>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -5734,6 +7626,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M106" t="n">
+        <v>70000618971</v>
+      </c>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -5784,6 +7694,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>VIÚVO(A)</t>
+        </is>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M107" t="n">
+        <v>70000618972</v>
+      </c>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>PRB</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -5834,6 +7762,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M108" t="n">
+        <v>70000618973</v>
+      </c>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>PRB</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -5884,6 +7830,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M109" t="n">
+        <v>70000622457</v>
+      </c>
+      <c r="N109" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -5934,6 +7898,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M110" t="n">
+        <v>70000622458</v>
+      </c>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -5984,6 +7966,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M111" t="n">
+        <v>70000622459</v>
+      </c>
+      <c r="N111" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -6034,6 +8034,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M112" t="n">
+        <v>70000622460</v>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -6084,6 +8102,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M113" t="n">
+        <v>70000622461</v>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -6134,6 +8170,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M114" t="n">
+        <v>70000622462</v>
+      </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -6184,6 +8238,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M115" t="n">
+        <v>70000622463</v>
+      </c>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -6234,6 +8306,24 @@
           <t>ENSINO MÉDIO INCOMPLETO</t>
         </is>
       </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M116" t="n">
+        <v>70000622464</v>
+      </c>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -6284,6 +8374,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M117" t="n">
+        <v>70000622465</v>
+      </c>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>PMN</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -6334,6 +8442,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M118" t="n">
+        <v>70000622466</v>
+      </c>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>PMN</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -6384,6 +8510,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>VIÚVO(A)</t>
+        </is>
+      </c>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M119" t="n">
+        <v>70000622467</v>
+      </c>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>PMN</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -6434,6 +8578,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M120" t="n">
+        <v>70000622468</v>
+      </c>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>PMN</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -6484,6 +8646,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M121" t="n">
+        <v>70000622469</v>
+      </c>
+      <c r="N121" t="inlineStr">
+        <is>
+          <t>PMN</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -6534,6 +8714,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M122" t="n">
+        <v>70000622470</v>
+      </c>
+      <c r="N122" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -6584,6 +8782,24 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="M123" t="n">
+        <v>70000622471</v>
+      </c>
+      <c r="N123" t="inlineStr">
+        <is>
+          <t>PMB</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -6634,6 +8850,24 @@
           <t>ENSINO MÉDIO INCOMPLETO</t>
         </is>
       </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L124" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M124" t="n">
+        <v>70000622472</v>
+      </c>
+      <c r="N124" t="inlineStr">
+        <is>
+          <t>PMB</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -6684,6 +8918,24 @@
           <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
         </is>
       </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M125" t="n">
+        <v>70000624319</v>
+      </c>
+      <c r="N125" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -6734,6 +8986,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M126" t="n">
+        <v>70000624320</v>
+      </c>
+      <c r="N126" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -6784,6 +9054,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M127" t="n">
+        <v>70000624321</v>
+      </c>
+      <c r="N127" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -6834,6 +9122,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L128" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M128" t="n">
+        <v>70000624322</v>
+      </c>
+      <c r="N128" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -6884,6 +9190,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L129" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M129" t="n">
+        <v>70000624323</v>
+      </c>
+      <c r="N129" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -6934,6 +9258,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L130" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M130" t="n">
+        <v>70000624324</v>
+      </c>
+      <c r="N130" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -6984,6 +9326,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M131" t="n">
+        <v>70000624325</v>
+      </c>
+      <c r="N131" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -7034,6 +9394,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M132" t="n">
+        <v>70000624326</v>
+      </c>
+      <c r="N132" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -7084,6 +9462,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L133" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M133" t="n">
+        <v>70000624327</v>
+      </c>
+      <c r="N133" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -7134,6 +9530,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L134" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M134" t="n">
+        <v>70000624328</v>
+      </c>
+      <c r="N134" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -7184,6 +9598,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L135" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M135" t="n">
+        <v>70000624329</v>
+      </c>
+      <c r="N135" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -7234,6 +9666,24 @@
           <t>ENSINO MÉDIO INCOMPLETO</t>
         </is>
       </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L136" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M136" t="n">
+        <v>70000624330</v>
+      </c>
+      <c r="N136" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -7284,6 +9734,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L137" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M137" t="n">
+        <v>70000624331</v>
+      </c>
+      <c r="N137" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -7334,6 +9802,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L138" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M138" t="n">
+        <v>70000624613</v>
+      </c>
+      <c r="N138" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -7384,6 +9870,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L139" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M139" t="n">
+        <v>70000624614</v>
+      </c>
+      <c r="N139" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -7434,6 +9938,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L140" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M140" t="n">
+        <v>70000624615</v>
+      </c>
+      <c r="N140" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -7484,6 +10006,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L141" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M141" t="n">
+        <v>70000624616</v>
+      </c>
+      <c r="N141" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -7534,6 +10074,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L142" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M142" t="n">
+        <v>70000624617</v>
+      </c>
+      <c r="N142" t="inlineStr">
+        <is>
+          <t>PATRIOTA</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -7584,6 +10142,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L143" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M143" t="n">
+        <v>70000624618</v>
+      </c>
+      <c r="N143" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -7634,6 +10210,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L144" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M144" t="n">
+        <v>70000624619</v>
+      </c>
+      <c r="N144" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -7684,6 +10278,24 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L145" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="M145" t="n">
+        <v>70000624620</v>
+      </c>
+      <c r="N145" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -7734,6 +10346,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L146" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M146" t="n">
+        <v>70000624621</v>
+      </c>
+      <c r="N146" t="inlineStr">
+        <is>
+          <t>PTC</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -7784,6 +10414,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L147" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M147" t="n">
+        <v>70000624622</v>
+      </c>
+      <c r="N147" t="inlineStr">
+        <is>
+          <t>PTC</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -7834,6 +10482,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L148" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M148" t="n">
+        <v>70000624623</v>
+      </c>
+      <c r="N148" t="inlineStr">
+        <is>
+          <t>PTC</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -7884,6 +10550,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L149" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M149" t="n">
+        <v>70000624624</v>
+      </c>
+      <c r="N149" t="inlineStr">
+        <is>
+          <t>PTC</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -7934,6 +10618,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L150" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M150" t="n">
+        <v>70000624625</v>
+      </c>
+      <c r="N150" t="inlineStr">
+        <is>
+          <t>PTC</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -7984,6 +10686,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L151" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M151" t="n">
+        <v>70000624626</v>
+      </c>
+      <c r="N151" t="inlineStr">
+        <is>
+          <t>PTC</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -8034,6 +10754,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L152" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M152" t="n">
+        <v>70000624627</v>
+      </c>
+      <c r="N152" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -8084,6 +10822,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M153" t="n">
+        <v>70000624628</v>
+      </c>
+      <c r="N153" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -8134,6 +10890,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M154" t="n">
+        <v>70000625523</v>
+      </c>
+      <c r="N154" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -8184,6 +10958,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>SEPARADO(A) JUDICIALMENTE</t>
+        </is>
+      </c>
+      <c r="L155" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M155" t="n">
+        <v>70000625524</v>
+      </c>
+      <c r="N155" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -8234,6 +11026,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L156" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M156" t="n">
+        <v>70000625525</v>
+      </c>
+      <c r="N156" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -8284,6 +11094,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L157" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M157" t="n">
+        <v>70000625526</v>
+      </c>
+      <c r="N157" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -8334,6 +11162,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L158" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M158" t="n">
+        <v>70000625527</v>
+      </c>
+      <c r="N158" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -8384,6 +11230,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L159" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M159" t="n">
+        <v>70000625528</v>
+      </c>
+      <c r="N159" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -8434,6 +11298,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L160" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M160" t="n">
+        <v>70000625529</v>
+      </c>
+      <c r="N160" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -8484,6 +11366,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L161" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M161" t="n">
+        <v>70000625530</v>
+      </c>
+      <c r="N161" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -8534,6 +11434,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L162" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M162" t="n">
+        <v>70000625531</v>
+      </c>
+      <c r="N162" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -8584,6 +11502,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L163" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M163" t="n">
+        <v>70000625532</v>
+      </c>
+      <c r="N163" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -8634,6 +11570,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L164" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M164" t="n">
+        <v>70000625533</v>
+      </c>
+      <c r="N164" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -8684,6 +11638,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L165" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M165" t="n">
+        <v>70000625534</v>
+      </c>
+      <c r="N165" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -8734,6 +11706,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L166" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M166" t="n">
+        <v>70000625535</v>
+      </c>
+      <c r="N166" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -8784,6 +11774,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L167" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M167" t="n">
+        <v>70000625536</v>
+      </c>
+      <c r="N167" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -8834,6 +11842,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L168" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M168" t="n">
+        <v>70000625537</v>
+      </c>
+      <c r="N168" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -8884,6 +11910,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L169" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M169" t="n">
+        <v>70000625538</v>
+      </c>
+      <c r="N169" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -8934,6 +11978,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L170" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M170" t="n">
+        <v>70000627341</v>
+      </c>
+      <c r="N170" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -8984,6 +12046,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L171" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M171" t="n">
+        <v>70000627342</v>
+      </c>
+      <c r="N171" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -9034,6 +12114,24 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="M172" t="n">
+        <v>70000627343</v>
+      </c>
+      <c r="N172" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -9084,6 +12182,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M173" t="n">
+        <v>70000627344</v>
+      </c>
+      <c r="N173" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -9134,6 +12250,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M174" t="n">
+        <v>70000627345</v>
+      </c>
+      <c r="N174" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -9184,6 +12318,24 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L175" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="M175" t="n">
+        <v>70000627346</v>
+      </c>
+      <c r="N175" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -9234,6 +12386,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L176" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M176" t="n">
+        <v>70000627347</v>
+      </c>
+      <c r="N176" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -9284,6 +12454,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L177" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M177" t="n">
+        <v>70000627348</v>
+      </c>
+      <c r="N177" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -9334,6 +12522,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L178" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M178" t="n">
+        <v>70000627349</v>
+      </c>
+      <c r="N178" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -9384,6 +12590,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L179" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M179" t="n">
+        <v>70000627350</v>
+      </c>
+      <c r="N179" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -9434,6 +12658,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L180" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M180" t="n">
+        <v>70000627351</v>
+      </c>
+      <c r="N180" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -9484,6 +12726,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L181" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M181" t="n">
+        <v>70000627352</v>
+      </c>
+      <c r="N181" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -9534,6 +12794,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L182" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M182" t="n">
+        <v>70000627353</v>
+      </c>
+      <c r="N182" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -9584,6 +12862,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L183" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M183" t="n">
+        <v>70000627354</v>
+      </c>
+      <c r="N183" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -9634,6 +12930,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L184" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M184" t="n">
+        <v>70000628275</v>
+      </c>
+      <c r="N184" t="inlineStr">
+        <is>
+          <t>PC do B</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -9684,6 +12998,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L185" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M185" t="n">
+        <v>70000628472</v>
+      </c>
+      <c r="N185" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -9734,6 +13066,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L186" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M186" t="n">
+        <v>70000629287</v>
+      </c>
+      <c r="N186" t="inlineStr">
+        <is>
+          <t>PMN</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -9784,6 +13134,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L187" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M187" t="n">
+        <v>70000629549</v>
+      </c>
+      <c r="N187" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -9834,6 +13202,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L188" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M188" t="n">
+        <v>70000629596</v>
+      </c>
+      <c r="N188" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -9884,6 +13270,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L189" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M189" t="n">
+        <v>70000629607</v>
+      </c>
+      <c r="N189" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -9934,6 +13338,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L190" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M190" t="n">
+        <v>70000629898</v>
+      </c>
+      <c r="N190" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -9984,6 +13406,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L191" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M191" t="n">
+        <v>70000630009</v>
+      </c>
+      <c r="N191" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -10032,6 +13472,24 @@
       <c r="J192" t="inlineStr">
         <is>
           <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L192" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M192" t="n">
+        <v>70000630086</v>
+      </c>
+      <c r="N192" t="inlineStr">
+        <is>
+          <t>PRB</t>
         </is>
       </c>
     </row>

</xml_diff>